<commit_message>
socio dempgraphic - psychological distress
</commit_message>
<xml_diff>
--- a/Key.xlsx
+++ b/Key.xlsx
@@ -110,7 +110,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="ＭＳ Ｐゴシック"/>
         <family val="2"/>
       </rPr>
@@ -119,7 +119,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -271,7 +271,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,13 +282,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -326,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -340,11 +334,8 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -657,8 +648,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="86.14785714285713" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="86.14785714285713" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -697,7 +688,7 @@
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>